<commit_message>
:presentation pdf/pptx + modif graph resultats
</commit_message>
<xml_diff>
--- a/results/Analyse_surface_prot_DSSP_MOI.xlsx
+++ b/results/Analyse_surface_prot_DSSP_MOI.xlsx
@@ -8,44 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victor/Documents/Master 2/projet cours/2022_M2-BI_Projet_court/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE7B3C1-F231-7045-A1C0-97C87F1E43F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0833FC-14F0-634B-9464-D838E37CFE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29100" windowHeight="18880" xr2:uid="{43BBE4B3-2D12-2D49-A63A-7920700C7CC9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29020" windowHeight="18880" xr2:uid="{43BBE4B3-2D12-2D49-A63A-7920700C7CC9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="EN" sheetId="1" r:id="rId1"/>
+    <sheet name="FR" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$6:$F$6</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">Feuil1!$B$7:$B$13</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Feuil1!$C$6</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Feuil1!$D$7:$D$13</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Feuil1!$B$7:$B$13</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Feuil1!$C$6</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Feuil1!$C$7:$C$13</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Feuil1!$D$6</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Feuil1!$D$7:$D$13</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Feuil1!$B$7:$B$13</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Feuil1!$C$6</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Feuil1!$C$7:$C$13</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Feuil1!$D$6</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Feuil1!$C$7:$C$13</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Feuil1!$D$7:$D$13</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Feuil1!$A$7:$A$13</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Feuil1!$B$6</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Feuil1!$B$7:$B$13</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Feuil1!$B$7:$B$13</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Feuil1!$C$6</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Feuil1!$C$7:$C$13</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Feuil1!$B$7:$B$13</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Feuil1!$C$6</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Feuil1!$C$7:$C$13</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Feuil1!$B$7:$B$13</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Feuil1!$C$6</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Feuil1!$C$7:$C$13</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Feuil1!$D$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EN!$B$6:$F$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FR!$B$6:$F$6</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -65,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>8dev</t>
   </si>
@@ -102,14 +77,23 @@
   <si>
     <t>SASCM</t>
   </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Standar-deviaiton</t>
+  </si>
+  <si>
+    <t>% error</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="179" formatCode="0.0"/>
-    <numFmt numFmtId="180" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -311,10 +295,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -326,13 +310,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -366,6 +350,1849 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>ASA of several proteins obtained</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> with </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>two programs</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> : </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>DSSP and SASCM </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EN!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SASCM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>EN!$E$7:$E$13</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>109.29749516800462</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>98.747461992701432</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>445.61869350376276</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>872.71118934043488</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3065.2725411046222</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6391.5240530095762</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>6324.1509188981227</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>EN!$E$7:$E$13</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>109.29749516800462</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>98.747461992701432</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>445.61869350376276</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>872.71118934043488</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3065.2725411046222</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6391.5240530095762</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>6324.1509188981227</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>EN!$B$7:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6a5j</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3i40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8d23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7u52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7r4h</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7pbp</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8dev</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EN!$C$7:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1710.57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3297.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18335.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33308.800000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75704.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>81980.02</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>119617.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-06A4-384B-BE7A-B8374BFDC49E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EN!$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DSSP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>EN!$B$7:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6a5j</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3i40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8d23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7u52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7r4h</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7pbp</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8dev</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EN!$D$7:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1556</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3437</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18966</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34543</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80039</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128561</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-06A4-384B-BE7A-B8374BFDC49E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="513441199"/>
+        <c:axId val="513445119"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="513441199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="513445119"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="513445119"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1200"/>
+                  <a:t>ASA in </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1200" b="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Å in</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1200" b="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t> log10</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR" sz="1200" b="0">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="513441199"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="10"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Correlation between DSSP and SASCM</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.4828875774387599E-2"/>
+                  <c:y val="-6.7136977937308981E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{095AC0D1-3A02-F84B-B8A9-6081C820489E}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-022B-7B4D-8867-2D542B0F8920}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.7539340723862646E-2"/>
+                  <c:y val="-6.1033616306643305E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{213928B8-94A4-AE48-A21D-B39D1693A264}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-022B-7B4D-8867-2D542B0F8920}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{D128F9FA-8C9E-3D45-B60A-D43CDE51D756}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-022B-7B4D-8867-2D542B0F8920}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{AD33C1DC-9D55-9647-8DFE-AF7B43B42351}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-022B-7B4D-8867-2D542B0F8920}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B05EE43A-1C8A-4B4B-A06A-1CD6C54F7D9C}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-022B-7B4D-8867-2D542B0F8920}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0EABF1E4-DFE4-804F-9B28-9D30AC89F00D}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-022B-7B4D-8867-2D542B0F8920}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C3560BD3-1B65-CE44-AC6F-20623A14E82F}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
+                      <a:pPr/>
+                      <a:t>[PLAGECELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-022B-7B4D-8867-2D542B0F8920}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.18149789815562087"/>
+                  <c:y val="9.4342592261081604E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>EN!$C$7:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1710.57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3297.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18335.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33308.800000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75704.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>81980.02</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>119617.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>EN!$D$7:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1556</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3437</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18966</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34543</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80039</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91019</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128561</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>EN!$B$7:$B$13</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>6a5j</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3i40</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8d23</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7u52</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7r4h</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7pbp</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>8dev</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-022B-7B4D-8867-2D542B0F8920}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1542617903"/>
+        <c:axId val="1542625295"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1542617903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1200" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>ASA in Å (SASCM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR" sz="1200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1542625295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1542625295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1200" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>ASA in Å (DSSP)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR" sz="1200">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1542617903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Error rate per protein</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>EN!$B$7:$C$13</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="7"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1710,6</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3297,4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>18335,8</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>33308,8</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>75704,1</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>81980,0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>119617,3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>6a5j</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3i40</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8d23</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7u52</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7r4h</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7pbp</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>8dev</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EN!$F$7:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>9.9338046272493527E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0631364562118154E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.322788147210802E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5729380771791594E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.4160471770012084E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9308715762642927E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9567753828921663E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0DF9-A04F-AC5E-4232D7DF291C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2076130351"/>
+        <c:axId val="2076174655"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2076130351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2076174655"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2076174655"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2076130351"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -451,7 +2278,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$C$6</c:f>
+              <c:f>FR!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -476,7 +2303,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Feuil1!$E$7:$E$13</c:f>
+                <c:f>FR!$E$7:$E$13</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
@@ -506,7 +2333,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Feuil1!$E$7:$E$13</c:f>
+                <c:f>FR!$E$7:$E$13</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
@@ -550,7 +2377,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$B$7:$B$13</c:f>
+              <c:f>FR!$B$7:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -579,7 +2406,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$C$7:$C$13</c:f>
+              <c:f>FR!$C$7:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -609,7 +2436,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-06A4-384B-BE7A-B8374BFDC49E}"/>
+              <c16:uniqueId val="{00000000-6319-B544-B499-DBFC4A9F2332}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -618,7 +2445,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$D$6</c:f>
+              <c:f>FR!$D$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -639,7 +2466,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$B$7:$B$13</c:f>
+              <c:f>FR!$B$7:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -668,7 +2495,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$D$7:$D$13</c:f>
+              <c:f>FR!$D$7:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -698,7 +2525,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-06A4-384B-BE7A-B8374BFDC49E}"/>
+              <c16:uniqueId val="{00000001-6319-B544-B499-DBFC4A9F2332}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -999,7 +2826,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -1118,7 +2945,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{033A37ED-B92C-B041-A378-3CF821CC0392}" type="CELLRANGE">
+                    <a:fld id="{5438C5AC-B74A-4A44-BB1D-ABEDAA7466A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1139,7 +2966,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-022B-7B4D-8867-2D542B0F8920}"/>
+                  <c16:uniqueId val="{00000000-0BF6-B348-A93D-4C34052EBAFB}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1156,7 +2983,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B1F0C5E4-A8E2-B144-9111-86C5540F1F2B}" type="CELLRANGE">
+                    <a:fld id="{21022FC7-D1CB-4A47-BC7F-8A87C437EDA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1177,7 +3004,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-022B-7B4D-8867-2D542B0F8920}"/>
+                  <c16:uniqueId val="{00000001-0BF6-B348-A93D-4C34052EBAFB}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1188,8 +3015,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{318924A2-C3DF-D84B-AED9-EF53A75955C2}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{38F33A10-07DE-B940-8688-B01EBCE2F5C7}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -1210,7 +3037,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-022B-7B4D-8867-2D542B0F8920}"/>
+                  <c16:uniqueId val="{00000002-0BF6-B348-A93D-4C34052EBAFB}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1221,8 +3048,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2417DB31-609F-334D-B52A-A8A54A01C1D1}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{A37A34AE-1339-6B44-B476-C4D8EC16CE31}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -1243,7 +3070,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-022B-7B4D-8867-2D542B0F8920}"/>
+                  <c16:uniqueId val="{00000003-0BF6-B348-A93D-4C34052EBAFB}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1254,8 +3081,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2DF74AA6-0F23-D94C-BF58-00D6E9B561BB}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{34299EC3-15C0-454C-96FA-650728E122A7}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -1276,7 +3103,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-022B-7B4D-8867-2D542B0F8920}"/>
+                  <c16:uniqueId val="{00000004-0BF6-B348-A93D-4C34052EBAFB}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1287,8 +3114,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91E70247-B2B1-F34C-A0E3-99FC229F21AD}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{BCF875D0-252A-EA40-B6DC-E5C54E19D77D}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -1309,7 +3136,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-022B-7B4D-8867-2D542B0F8920}"/>
+                  <c16:uniqueId val="{00000005-0BF6-B348-A93D-4C34052EBAFB}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1320,8 +3147,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{018F9690-DAC6-824B-8F61-48E07F418FCF}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{20B90FDE-58DA-7D4A-A10E-CFF197D3088F}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -1342,7 +3169,7 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-022B-7B4D-8867-2D542B0F8920}"/>
+                  <c16:uniqueId val="{00000006-0BF6-B348-A93D-4C34052EBAFB}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1457,7 +3284,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$C$7:$C$13</c:f>
+              <c:f>FR!$C$7:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1487,7 +3314,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$D$7:$D$13</c:f>
+              <c:f>FR!$D$7:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1519,7 +3346,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Feuil1!$B$7:$B$13</c15:f>
+                <c15:f>FR!$B$7:$B$13</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
@@ -1547,7 +3374,7 @@
               </c15:datalabelsRange>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-022B-7B4D-8867-2D542B0F8920}"/>
+              <c16:uniqueId val="{00000008-0BF6-B348-A93D-4C34052EBAFB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1858,7 +3685,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -1949,7 +3776,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Feuil1!$B$7:$C$13</c:f>
+              <c:f>FR!$B$7:$C$13</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="7"/>
                 <c:lvl>
@@ -2003,7 +3830,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$F$7:$F$13</c:f>
+              <c:f>FR!$F$7:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2033,7 +3860,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0DF9-A04F-AC5E-4232D7DF291C}"/>
+              <c16:uniqueId val="{00000000-0B6B-844E-AEB2-9D18F1DA0E87}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2075,7 +3902,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2322,6 +4149,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3342,6 +5289,1528 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3924,16 +7393,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1258887</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>178594</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>692944</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>186531</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3944,7 +7413,128 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28113</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9410</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>813506</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>136410</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5DC989D-16C3-0849-9E64-6E76D10AF3AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>12968</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>6823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>785810</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>131940</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5586F11C-4A5A-AF4A-A244-7AF9DEF43629}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1258887</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>178594</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>692944</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>186531</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3853534B-26CE-2F4D-B0F3-9EDB4F4A51E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4260,8 +7850,206 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032E2E88-BD01-5842-89D6-BDB464D9DA6A}">
   <dimension ref="B5:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1710.57</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1556</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" ref="E7:E13" si="0">STDEV(C7,D7)</f>
+        <v>109.29749516800462</v>
+      </c>
+      <c r="F7" s="9">
+        <f>ABS(C7-D7)/D7</f>
+        <v>9.9338046272493527E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3297.35</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3437</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>98.747461992701432</v>
+      </c>
+      <c r="F8" s="9">
+        <f t="shared" ref="F8:F13" si="1">ABS(C8-D8)/D8</f>
+        <v>4.0631364562118154E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>18335.8</v>
+      </c>
+      <c r="D9" s="2">
+        <v>18966</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>445.61869350376276</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" si="1"/>
+        <v>3.322788147210802E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3">
+        <v>33308.800000000003</v>
+      </c>
+      <c r="D10" s="2">
+        <v>34543</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>872.71118934043488</v>
+      </c>
+      <c r="F10" s="9">
+        <f t="shared" si="1"/>
+        <v>3.5729380771791594E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>75704.05</v>
+      </c>
+      <c r="D11" s="2">
+        <v>80039</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>3065.2725411046222</v>
+      </c>
+      <c r="F11" s="9">
+        <f t="shared" si="1"/>
+        <v>5.4160471770012084E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3">
+        <v>81980.02</v>
+      </c>
+      <c r="D12" s="2">
+        <v>91019</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>6391.5240530095762</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="1"/>
+        <v>9.9308715762642927E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>119617.3</v>
+      </c>
+      <c r="D13" s="2">
+        <v>128561</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>6324.1509188981227</v>
+      </c>
+      <c r="F13" s="9">
+        <f t="shared" si="1"/>
+        <v>6.9567753828921663E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J28" s="1"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B6:F6" xr:uid="{032E2E88-BD01-5842-89D6-BDB464D9DA6A}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F707A547-52A7-3743-A06A-BE996ADE1700}">
+  <dimension ref="B5:J28"/>
+  <sheetViews>
+    <sheetView zoomScale="64" workbookViewId="0">
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4303,7 +8091,7 @@
         <v>1556</v>
       </c>
       <c r="E7" s="8">
-        <f>STDEV(C7,D7)</f>
+        <f t="shared" ref="E7:E13" si="0">STDEV(C7,D7)</f>
         <v>109.29749516800462</v>
       </c>
       <c r="F7" s="9">
@@ -4322,11 +8110,11 @@
         <v>3437</v>
       </c>
       <c r="E8" s="2">
-        <f>STDEV(C8,D8)</f>
+        <f t="shared" si="0"/>
         <v>98.747461992701432</v>
       </c>
       <c r="F8" s="9">
-        <f t="shared" ref="F8:F13" si="0">ABS(C8-D8)/D8</f>
+        <f t="shared" ref="F8:F13" si="1">ABS(C8-D8)/D8</f>
         <v>4.0631364562118154E-2</v>
       </c>
     </row>
@@ -4341,11 +8129,11 @@
         <v>18966</v>
       </c>
       <c r="E9" s="2">
-        <f>STDEV(C9,D9)</f>
+        <f t="shared" si="0"/>
         <v>445.61869350376276</v>
       </c>
       <c r="F9" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.322788147210802E-2</v>
       </c>
     </row>
@@ -4360,11 +8148,11 @@
         <v>34543</v>
       </c>
       <c r="E10" s="2">
-        <f>STDEV(C10,D10)</f>
+        <f t="shared" si="0"/>
         <v>872.71118934043488</v>
       </c>
       <c r="F10" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.5729380771791594E-2</v>
       </c>
     </row>
@@ -4379,11 +8167,11 @@
         <v>80039</v>
       </c>
       <c r="E11" s="2">
-        <f>STDEV(C11,D11)</f>
+        <f t="shared" si="0"/>
         <v>3065.2725411046222</v>
       </c>
       <c r="F11" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.4160471770012084E-2</v>
       </c>
     </row>
@@ -4398,11 +8186,11 @@
         <v>91019</v>
       </c>
       <c r="E12" s="2">
-        <f>STDEV(C12,D12)</f>
+        <f t="shared" si="0"/>
         <v>6391.5240530095762</v>
       </c>
       <c r="F12" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.9308715762642927E-2</v>
       </c>
     </row>
@@ -4417,11 +8205,11 @@
         <v>128561</v>
       </c>
       <c r="E13" s="2">
-        <f>STDEV(C13,D13)</f>
+        <f t="shared" si="0"/>
         <v>6324.1509188981227</v>
       </c>
       <c r="F13" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.9567753828921663E-2</v>
       </c>
     </row>

</xml_diff>